<commit_message>
lme lchsa lchltd kdpw
</commit_message>
<xml_diff>
--- a/data/ccg/ccg-Q1-2017.xlsx
+++ b/data/ccg/ccg-Q1-2017.xlsx
@@ -92,10 +92,10 @@
     <t>23.1.2.OTC</t>
   </si>
   <si>
+    <t>23.1.2.ETD</t>
+  </si>
+  <si>
     <t>23.2.1.OTC</t>
-  </si>
-  <si>
-    <t>23.1.2.ETD</t>
   </si>
   <si>
     <t>23.2.1.ETD</t>
@@ -631,10 +631,10 @@
         <v>0</v>
       </c>
       <c r="AA2" t="n">
-        <v>0</v>
+        <v>80009923076</v>
       </c>
       <c r="AB2" t="n">
-        <v>80009923076</v>
+        <v>0</v>
       </c>
       <c r="AC2" t="n">
         <v>33751531154</v>
@@ -712,10 +712,10 @@
         <v>0</v>
       </c>
       <c r="AA3" t="n">
-        <v>0</v>
+        <v>2147479381</v>
       </c>
       <c r="AB3" t="n">
-        <v>2147479381</v>
+        <v>0</v>
       </c>
       <c r="AC3" t="n">
         <v>753150847869</v>
@@ -793,10 +793,10 @@
         <v>0</v>
       </c>
       <c r="AA4" t="n">
-        <v>0</v>
+        <v>6305862669</v>
       </c>
       <c r="AB4" t="n">
-        <v>6305862669</v>
+        <v>0</v>
       </c>
       <c r="AC4" t="n">
         <v>140388271</v>
@@ -874,10 +874,10 @@
         <v>0</v>
       </c>
       <c r="AA5" t="n">
-        <v>0</v>
+        <v>822497</v>
       </c>
       <c r="AB5" t="n">
-        <v>822497</v>
+        <v>0</v>
       </c>
       <c r="AC5" t="n">
         <v>1509000</v>

</xml_diff>